<commit_message>
Inclusao de modelo de rede neural densa baseado no tensorflow. Correcao do nome do modelo que aparece na legenda da curva roc.
</commit_message>
<xml_diff>
--- a/Results/all_results.xlsx
+++ b/Results/all_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,25 +490,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9649</v>
+        <v>0.9552</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9637</v>
+        <v>0.9488</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9663</v>
+        <v>0.9623</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.965</v>
+        <v>0.9555</v>
       </c>
     </row>
     <row r="3">
@@ -521,25 +521,25 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9549</v>
+        <v>0.9498</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9754</v>
+        <v>0.9647</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9334</v>
+        <v>0.9338</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9539</v>
+        <v>0.949</v>
       </c>
     </row>
     <row r="4">
@@ -549,28 +549,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8518</v>
+        <v>0.8494</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8326</v>
+        <v>0.837</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8961</v>
+        <v>0.8957000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8657</v>
+        <v>0.8799</v>
       </c>
       <c r="F4" t="n">
-        <v>0.796</v>
+        <v>0.7907999999999999</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7873</v>
+        <v>0.7806</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8431</v>
+        <v>0.84</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8247</v>
+        <v>0.8273</v>
       </c>
     </row>
     <row r="5">
@@ -580,28 +580,59 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8832</v>
+        <v>0.8831</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8321</v>
+        <v>0.8337</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9215</v>
+        <v>0.9256</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8628</v>
+        <v>0.8767</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8378</v>
+        <v>0.8333</v>
       </c>
       <c r="G5" t="n">
-        <v>0.79</v>
+        <v>0.7766</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8777</v>
+        <v>0.877</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8248</v>
+        <v>0.8236</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Sequential</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.822</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.8257</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.8653</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.8695000000000001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.7628</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.7664</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.8108</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.8147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>